<commit_message>
added new indicators to FT list
</commit_message>
<xml_diff>
--- a/data/LA_FingerTips_Indicators.xlsx
+++ b/data/LA_FingerTips_Indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://birminghamcitycouncil-my.sharepoint.com/personal/david_ellis_birmingham_gov_uk/Documents/Documents/Main work/Outcome Framework/BSOL_Outcomes_Framework/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="8_{A321533F-7BC8-4AA5-876C-441F25B49F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9431E6ED-67D5-4B56-8628-65B07D827C56}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="8_{A321533F-7BC8-4AA5-876C-441F25B49F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFBAF283-9C8A-4569-A53C-267F3C66A7B6}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E792575E-E25C-4FCA-9324-1D04337FED20}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{E792575E-E25C-4FCA-9324-1D04337FED20}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>IndicatorID</t>
   </si>
@@ -701,9 +701,6 @@
     <xf numFmtId="0" fontId="13" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -715,6 +712,9 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -817,8 +817,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}" name="Table1" displayName="Table1" ref="A1:C14" totalsRowShown="0">
-  <autoFilter ref="A1:C14" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}" name="Table1" displayName="Table1" ref="A1:C16" totalsRowShown="0">
+  <autoFilter ref="A1:C16" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{10CB49F6-EA4D-4880-BF95-DC071EFD0853}" name="IndicatorID" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{DAADBE55-31EA-4A87-8258-333CF52E3BA3}" name="FingerTips_id" dataDxfId="1"/>
@@ -1158,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6BDC081-4CB1-469F-9897-DEC94E260883}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1174,10 +1174,10 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="13"/>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1189,18 +1189,18 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="52.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1214,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7D95AE-3944-4DF5-9B38-8E42A110E601}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1379,6 +1379,28 @@
       </c>
       <c r="C14" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>34</v>
+      </c>
+      <c r="B15" s="1">
+        <v>92781</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>55</v>
+      </c>
+      <c r="B16" s="1">
+        <v>93605</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated rate type for percentages
</commit_message>
<xml_diff>
--- a/data/LA_FingerTips_Indicators.xlsx
+++ b/data/LA_FingerTips_Indicators.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="91" documentId="8_{A321533F-7BC8-4AA5-876C-441F25B49F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFBAF283-9C8A-4569-A53C-267F3C66A7B6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{E792575E-E25C-4FCA-9324-1D04337FED20}"/>
+    <workbookView minimized="1" xWindow="-3504" yWindow="7104" windowWidth="17280" windowHeight="10056" activeTab="1" xr2:uid="{E792575E-E25C-4FCA-9324-1D04337FED20}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -1217,7 +1217,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Now using PCN-to-locality lookup, updated Byar's CI, only calculating ICB value if both Solihull and Birmingham value present
</commit_message>
<xml_diff>
--- a/data/LA_FingerTips_Indicators.xlsx
+++ b/data/LA_FingerTips_Indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://birminghamcitycouncil-my.sharepoint.com/personal/david_ellis_birmingham_gov_uk/Documents/Documents/Main work/Outcome Framework/BSOL_Outcomes_Framework/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="8_{A321533F-7BC8-4AA5-876C-441F25B49F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFBAF283-9C8A-4569-A53C-267F3C66A7B6}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="8_{A321533F-7BC8-4AA5-876C-441F25B49F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33E391A0-7D36-4F7C-B086-D20C0C9E5552}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-3504" yWindow="7104" windowWidth="17280" windowHeight="10056" activeTab="1" xr2:uid="{E792575E-E25C-4FCA-9324-1D04337FED20}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{E792575E-E25C-4FCA-9324-1D04337FED20}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -819,6 +819,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}" name="Table1" displayName="Table1" ref="A1:C16" totalsRowShown="0">
   <autoFilter ref="A1:C16" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C16">
+    <sortCondition ref="A1:A16"/>
+  </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{10CB49F6-EA4D-4880-BF95-DC071EFD0853}" name="IndicatorID" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{DAADBE55-31EA-4A87-8258-333CF52E3BA3}" name="FingerTips_id" dataDxfId="1"/>
@@ -1217,7 +1220,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1239,22 +1242,22 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>15</v>
-      </c>
-      <c r="B2">
-        <v>41203</v>
+      <c r="A2" s="1">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>811</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>23</v>
-      </c>
-      <c r="B3">
-        <v>92254</v>
+      <c r="A3" s="1">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>30307</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1262,43 +1265,43 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B4">
-        <v>92601</v>
+        <v>41203</v>
       </c>
       <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1">
+        <v>90619</v>
+      </c>
+      <c r="C5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>47</v>
-      </c>
-      <c r="B5">
-        <v>93183</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>57</v>
-      </c>
-      <c r="B6">
-        <v>93675</v>
+      <c r="A6" s="1">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1">
+        <v>91340</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>811</v>
+      <c r="A7">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>92254</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -1306,21 +1309,21 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1">
-        <v>30307</v>
+        <v>92517</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>17</v>
-      </c>
-      <c r="B9" s="1">
-        <v>90619</v>
+      <c r="A9">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <v>92601</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -1328,10 +1331,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B10" s="1">
-        <v>91340</v>
+        <v>92781</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -1339,65 +1342,65 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1">
-        <v>92517</v>
+        <v>93085</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>44</v>
-      </c>
-      <c r="B12" s="1">
-        <v>93085</v>
+      <c r="A12" s="2">
+        <v>45</v>
+      </c>
+      <c r="B12" s="2">
+        <v>92588</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>111</v>
-      </c>
-      <c r="B13" s="1">
-        <v>22001</v>
+      <c r="A13">
+        <v>47</v>
+      </c>
+      <c r="B13">
+        <v>93183</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>45</v>
-      </c>
-      <c r="B14" s="2">
-        <v>92588</v>
+      <c r="A14" s="1">
+        <v>55</v>
+      </c>
+      <c r="B14" s="1">
+        <v>93605</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>34</v>
-      </c>
-      <c r="B15" s="1">
-        <v>92781</v>
+      <c r="A15">
+        <v>57</v>
+      </c>
+      <c r="B15">
+        <v>93675</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="B16" s="1">
-        <v>93605</v>
+        <v>22001</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Corrected FingerTips ID for indicator 45
</commit_message>
<xml_diff>
--- a/data/LA_FingerTips_Indicators.xlsx
+++ b/data/LA_FingerTips_Indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://birminghamcitycouncil-my.sharepoint.com/personal/david_ellis_birmingham_gov_uk/Documents/Documents/Main work/Outcome Framework/BSOL_Outcomes_Framework/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="8_{A321533F-7BC8-4AA5-876C-441F25B49F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33E391A0-7D36-4F7C-B086-D20C0C9E5552}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="8_{A321533F-7BC8-4AA5-876C-441F25B49F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD8D3A16-E940-4A7A-B672-7C4753B390DF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{E792575E-E25C-4FCA-9324-1D04337FED20}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>IndicatorID</t>
   </si>
@@ -70,7 +70,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +234,13 @@
     <font>
       <sz val="24"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -683,7 +690,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -713,6 +720,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -817,10 +825,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}" name="Table1" displayName="Table1" ref="A1:C16" totalsRowShown="0">
-  <autoFilter ref="A1:C16" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C16">
-    <sortCondition ref="A1:A16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}" name="Table1" displayName="Table1" ref="A1:C18" totalsRowShown="0">
+  <autoFilter ref="A1:C18" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C18">
+    <sortCondition ref="A1:A18"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{10CB49F6-EA4D-4880-BF95-DC071EFD0853}" name="IndicatorID" dataDxfId="2"/>
@@ -1177,10 +1185,10 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="14"/>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1217,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7D95AE-3944-4DF5-9B38-8E42A110E601}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1254,21 +1262,21 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>30307</v>
+        <v>20101</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>15</v>
-      </c>
-      <c r="B4">
-        <v>41203</v>
+      <c r="A4" s="1">
+        <v>7</v>
+      </c>
+      <c r="B4" s="13">
+        <v>20401</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1276,109 +1284,109 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1">
+        <v>30307</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>41203</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>17</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B7" s="1">
         <v>90619</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>20</v>
-      </c>
-      <c r="B6" s="1">
-        <v>91340</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>23</v>
-      </c>
-      <c r="B7">
-        <v>92254</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1">
-        <v>92517</v>
+        <v>91340</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B9">
-        <v>92601</v>
+        <v>92254</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1">
+        <v>92517</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <v>92601</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>34</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B12" s="1">
         <v>92781</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>44</v>
-      </c>
-      <c r="B11" s="1">
-        <v>93085</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>45</v>
-      </c>
-      <c r="B12" s="2">
-        <v>92588</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>47</v>
-      </c>
-      <c r="B13">
-        <v>93183</v>
+      <c r="A13" s="1">
+        <v>44</v>
+      </c>
+      <c r="B13" s="1">
+        <v>93085</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>55</v>
-      </c>
-      <c r="B14" s="1">
-        <v>93605</v>
+      <c r="A14" s="2">
+        <v>45</v>
+      </c>
+      <c r="B14" s="2">
+        <v>93088</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -1386,10 +1394,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B15">
-        <v>93675</v>
+        <v>93183</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -1397,12 +1405,34 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
+        <v>55</v>
+      </c>
+      <c r="B16" s="1">
+        <v>93605</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>57</v>
+      </c>
+      <c r="B17">
+        <v>93675</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>111</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B18" s="1">
         <v>22001</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new indicators for FingerTips extraction
</commit_message>
<xml_diff>
--- a/data/LA_FingerTips_Indicators.xlsx
+++ b/data/LA_FingerTips_Indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://birminghamcitycouncil-my.sharepoint.com/personal/david_ellis_birmingham_gov_uk/Documents/Documents/Main work/Outcome Framework/BSOL_Outcomes_Framework/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="8_{A321533F-7BC8-4AA5-876C-441F25B49F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD8D3A16-E940-4A7A-B672-7C4753B390DF}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="8_{A321533F-7BC8-4AA5-876C-441F25B49F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D44FE3BB-87F1-4E37-8D61-BAA0D6037616}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{E792575E-E25C-4FCA-9324-1D04337FED20}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
   <si>
     <t>IndicatorID</t>
   </si>
@@ -70,7 +70,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +245,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0B0C0C"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -439,7 +445,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -643,6 +649,15 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -690,7 +705,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -721,8 +736,21 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -825,10 +853,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}" name="Table1" displayName="Table1" ref="A1:C18" totalsRowShown="0">
-  <autoFilter ref="A1:C18" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C18">
-    <sortCondition ref="A1:A18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0">
+  <autoFilter ref="A1:C20" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C20">
+    <sortCondition ref="A1:A20"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{10CB49F6-EA4D-4880-BF95-DC071EFD0853}" name="IndicatorID" dataDxfId="2"/>
@@ -1185,10 +1213,10 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14"/>
+      <c r="B3" s="15"/>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1225,10 +1253,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7D95AE-3944-4DF5-9B38-8E42A110E601}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1261,10 +1289,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="A3" s="17">
         <v>6</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="17">
         <v>20101</v>
       </c>
       <c r="C3" t="s">
@@ -1327,44 +1355,44 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>23</v>
-      </c>
-      <c r="B9">
-        <v>92254</v>
+      <c r="A9" s="16">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1">
+        <v>91743</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>27</v>
-      </c>
-      <c r="B10" s="1">
-        <v>92517</v>
+      <c r="A10">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>92254</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="1">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1">
+        <v>92517</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>30</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>92601</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>34</v>
-      </c>
-      <c r="B12" s="1">
-        <v>92781</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -1372,67 +1400,89 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1">
+        <v>92781</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>44</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B14" s="1">
         <v>93085</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>45</v>
-      </c>
-      <c r="B14" s="2">
-        <v>93088</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>47</v>
-      </c>
-      <c r="B15">
-        <v>93183</v>
+      <c r="A15" s="2">
+        <v>45</v>
+      </c>
+      <c r="B15" s="2">
+        <v>93088</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>55</v>
-      </c>
-      <c r="B16" s="1">
-        <v>93605</v>
+      <c r="A16">
+        <v>47</v>
+      </c>
+      <c r="B16">
+        <v>93183</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>57</v>
-      </c>
-      <c r="B17">
-        <v>93675</v>
+      <c r="A17" s="1">
+        <v>55</v>
+      </c>
+      <c r="B17" s="1">
+        <v>93605</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+      <c r="A18">
+        <v>57</v>
+      </c>
+      <c r="B18">
+        <v>93675</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="14">
         <v>111</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B19" s="19">
         <v>22001</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="17">
+        <v>130</v>
+      </c>
+      <c r="B20" s="18">
+        <v>91819</v>
+      </c>
+      <c r="C20" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Highlighted and removed missing GP data for IDs 17, 20, and 34
</commit_message>
<xml_diff>
--- a/data/LA_FingerTips_Indicators.xlsx
+++ b/data/LA_FingerTips_Indicators.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1250,7 +1250,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added function to collect only England data and added indicator 71 to that list
</commit_message>
<xml_diff>
--- a/data/LA_FingerTips_Indicators.xlsx
+++ b/data/LA_FingerTips_Indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://birminghamcitycouncil-my.sharepoint.com/personal/david_ellis_birmingham_gov_uk/Documents/Documents/Main work/Outcome Framework/BSOL_Outcomes_Framework/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="122" documentId="8_{A321533F-7BC8-4AA5-876C-441F25B49F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B28AAE5-7124-4AA2-9081-700C28DA3504}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="8_{A321533F-7BC8-4AA5-876C-441F25B49F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83C616CD-01C6-435E-A56B-83BCFF75500B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{E792575E-E25C-4FCA-9324-1D04337FED20}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E792575E-E25C-4FCA-9324-1D04337FED20}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>IndicatorID</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>FingerTips Indicator List</t>
+  </si>
+  <si>
+    <t>England</t>
   </si>
 </sst>
 </file>
@@ -847,10 +850,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}" name="Table1" displayName="Table1" ref="A1:C19" totalsRowShown="0">
-  <autoFilter ref="A1:C19" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C19">
-    <sortCondition ref="A1:A19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0">
+  <autoFilter ref="A1:C20" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C20">
+    <sortCondition ref="A1:A20"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{10CB49F6-EA4D-4880-BF95-DC071EFD0853}" name="IndicatorID" dataDxfId="2"/>
@@ -862,8 +865,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{47B1D9EB-15EF-444F-BEB3-B96D3F28A878}" name="Table2" displayName="Table2" ref="A1:B8" totalsRowShown="0">
-  <autoFilter ref="A1:B8" xr:uid="{47B1D9EB-15EF-444F-BEB3-B96D3F28A878}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{47B1D9EB-15EF-444F-BEB3-B96D3F28A878}" name="Table2" displayName="Table2" ref="A1:B7" totalsRowShown="0">
+  <autoFilter ref="A1:B7" xr:uid="{47B1D9EB-15EF-444F-BEB3-B96D3F28A878}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1007C73B-93EE-4B09-AAC2-3766FAF8B28C}" name="IndicatorID"/>
     <tableColumn id="2" xr3:uid="{FEF03DA6-5215-4C5B-A495-FD5C3E88E8F7}" name="FingerTips_ID" dataDxfId="0"/>
@@ -1247,10 +1250,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7D95AE-3944-4DF5-9B38-8E42A110E601}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1459,13 +1462,24 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="14">
+      <c r="A19" s="1">
+        <v>71</v>
+      </c>
+      <c r="B19" s="1">
+        <v>91041</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="14">
         <v>111</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B20" s="16">
         <v>22001</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1482,10 +1496,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D640AEB9-8868-4341-BD1C-36C3E1E17A33}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1520,41 +1534,33 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="B4" s="5">
-        <v>91041</v>
+        <v>92962</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B5" s="5">
-        <v>92962</v>
+        <v>93012</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>119</v>
-      </c>
-      <c r="B6" s="5">
-        <v>93012</v>
+        <v>130</v>
+      </c>
+      <c r="B6" s="4">
+        <v>91819</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>130</v>
-      </c>
-      <c r="B7" s="4">
-        <v>91819</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
         <v>131</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B7" s="3">
         <v>90631</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated to pull LA and ICB data from FT for HC indicator (ID = 71)
</commit_message>
<xml_diff>
--- a/data/LA_FingerTips_Indicators.xlsx
+++ b/data/LA_FingerTips_Indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://birminghamcitycouncil-my.sharepoint.com/personal/david_ellis_birmingham_gov_uk/Documents/Documents/Main work/Outcome Framework/BSOL_Outcomes_Framework/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="8_{A321533F-7BC8-4AA5-876C-441F25B49F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83C616CD-01C6-435E-A56B-83BCFF75500B}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="8_{A321533F-7BC8-4AA5-876C-441F25B49F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{128313D9-D0AF-493D-BB21-0657E58D24A1}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E792575E-E25C-4FCA-9324-1D04337FED20}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E792575E-E25C-4FCA-9324-1D04337FED20}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
   <si>
     <t>IndicatorID</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>FingerTips Indicator List</t>
-  </si>
-  <si>
-    <t>England</t>
   </si>
 </sst>
 </file>
@@ -1252,8 +1249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7D95AE-3944-4DF5-9B38-8E42A110E601}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1469,7 +1466,7 @@
         <v>91041</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1498,8 +1495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D640AEB9-8868-4341-BD1C-36C3E1E17A33}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added indicator 131 into standardised FingerTips API pipeline
</commit_message>
<xml_diff>
--- a/data/LA_FingerTips_Indicators.xlsx
+++ b/data/LA_FingerTips_Indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://birminghamcitycouncil-my.sharepoint.com/personal/david_ellis_birmingham_gov_uk/Documents/Documents/Main work/Outcome Framework/BSOL_Outcomes_Framework/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="8_{A321533F-7BC8-4AA5-876C-441F25B49F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{128313D9-D0AF-493D-BB21-0657E58D24A1}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="8_{A321533F-7BC8-4AA5-876C-441F25B49F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4391DA2F-D5D9-447A-8204-95BE5758EEBC}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E792575E-E25C-4FCA-9324-1D04337FED20}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{E792575E-E25C-4FCA-9324-1D04337FED20}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
   <si>
     <t>IndicatorID</t>
   </si>
@@ -70,7 +70,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,13 +210,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0B0C0C"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -705,7 +698,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -713,37 +706,34 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -847,8 +837,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0">
-  <autoFilter ref="A1:C20" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}" name="Table1" displayName="Table1" ref="A1:C21" totalsRowShown="0">
+  <autoFilter ref="A1:C21" xr:uid="{189D5B51-557E-427E-8E6E-36CB4CF41561}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C20">
     <sortCondition ref="A1:A20"/>
   </sortState>
@@ -862,8 +852,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{47B1D9EB-15EF-444F-BEB3-B96D3F28A878}" name="Table2" displayName="Table2" ref="A1:B7" totalsRowShown="0">
-  <autoFilter ref="A1:B7" xr:uid="{47B1D9EB-15EF-444F-BEB3-B96D3F28A878}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{47B1D9EB-15EF-444F-BEB3-B96D3F28A878}" name="Table2" displayName="Table2" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6" xr:uid="{47B1D9EB-15EF-444F-BEB3-B96D3F28A878}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1007C73B-93EE-4B09-AAC2-3766FAF8B28C}" name="IndicatorID"/>
     <tableColumn id="2" xr3:uid="{FEF03DA6-5215-4C5B-A495-FD5C3E88E8F7}" name="FingerTips_ID" dataDxfId="0"/>
@@ -1202,38 +1192,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="17"/>
+      <c r="B3" s="16"/>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="52.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1247,10 +1237,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7D95AE-3944-4DF5-9B38-8E42A110E601}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1297,7 +1287,7 @@
       <c r="A4" s="1">
         <v>7</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>20401</v>
       </c>
       <c r="C4" t="s">
@@ -1349,7 +1339,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="15">
+      <c r="A9" s="14">
         <v>21</v>
       </c>
       <c r="B9" s="1">
@@ -1470,13 +1460,24 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="14">
+      <c r="A20" s="13">
         <v>111</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20" s="15">
         <v>22001</v>
       </c>
       <c r="C20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>131</v>
+      </c>
+      <c r="B21" s="1">
+        <v>90631</v>
+      </c>
+      <c r="C21" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1493,10 +1494,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D640AEB9-8868-4341-BD1C-36C3E1E17A33}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1517,7 +1518,7 @@
       <c r="A2">
         <v>8</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>20601</v>
       </c>
     </row>
@@ -1525,7 +1526,7 @@
       <c r="A3">
         <v>9</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>20602</v>
       </c>
     </row>
@@ -1533,7 +1534,7 @@
       <c r="A4">
         <v>118</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>92962</v>
       </c>
     </row>
@@ -1541,7 +1542,7 @@
       <c r="A5">
         <v>119</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>93012</v>
       </c>
     </row>
@@ -1549,16 +1550,8 @@
       <c r="A6">
         <v>130</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>91819</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>131</v>
-      </c>
-      <c r="B7" s="3">
-        <v>90631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>